<commit_message>
with new saved models
</commit_message>
<xml_diff>
--- a/summary_model_training.xlsx
+++ b/summary_model_training.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andreasoggia/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andreasoggia/code/asoggia/tails-and-whales/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BCB75573-6339-E246-9F5B-811DC230FC95}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ABF665D-3B0E-1241-9F5F-66D5D12416D4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="260" yWindow="500" windowWidth="27540" windowHeight="16940" xr2:uid="{7D70B26E-E1F8-C845-A8E2-BB9C89E3CB97}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="27540" windowHeight="16940" xr2:uid="{7D70B26E-E1F8-C845-A8E2-BB9C89E3CB97}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="58">
   <si>
     <t>model_1</t>
   </si>
@@ -42,12 +42,6 @@
     <t>couches additionelles</t>
   </si>
   <si>
-    <t>métrique</t>
-  </si>
-  <si>
-    <t>evaluate</t>
-  </si>
-  <si>
     <t>flatten + 2 denses (500)</t>
   </si>
   <si>
@@ -61,16 +55,183 @@
   </si>
   <si>
     <t>non :16</t>
+  </si>
+  <si>
+    <t>model_3</t>
+  </si>
+  <si>
+    <t>monitor</t>
+  </si>
+  <si>
+    <t>val_loss</t>
+  </si>
+  <si>
+    <t>val_accuracy</t>
+  </si>
+  <si>
+    <t>X_size</t>
+  </si>
+  <si>
+    <t>patience</t>
+  </si>
+  <si>
+    <t>evaluate sur test</t>
+  </si>
+  <si>
+    <t>epochs</t>
+  </si>
+  <si>
+    <t>model_4</t>
+  </si>
+  <si>
+    <t>Stopped manually at epoch 6</t>
+  </si>
+  <si>
+    <t>size X_test</t>
+  </si>
+  <si>
+    <t>model_5</t>
+  </si>
+  <si>
+    <t>X.shape</t>
+  </si>
+  <si>
+    <t>256,256,3</t>
+  </si>
+  <si>
+    <t>batch_size</t>
+  </si>
+  <si>
+    <t>Stopped</t>
+  </si>
+  <si>
+    <t>model_6</t>
+  </si>
+  <si>
+    <t>64,64,3</t>
+  </si>
+  <si>
+    <t>métrique: res sur X_val</t>
+  </si>
+  <si>
+    <t>accuracy : 90%</t>
+  </si>
+  <si>
+    <t>non : (19-3=16)</t>
+  </si>
+  <si>
+    <t>model_7</t>
+  </si>
+  <si>
+    <t>ALL</t>
+  </si>
+  <si>
+    <t>model_8</t>
+  </si>
+  <si>
+    <t>accuracy : 93,8%</t>
+  </si>
+  <si>
+    <t>accuracy : ?</t>
+  </si>
+  <si>
+    <t>EarlyStopping at epoch 9</t>
+  </si>
+  <si>
+    <t>accuracy : 89%</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>* need the X_test with the right shape</t>
+  </si>
+  <si>
+    <t>EarlyStopping at epoch 10</t>
+  </si>
+  <si>
+    <t>accuracy : 93%</t>
+  </si>
+  <si>
+    <t>mobilenetv2</t>
+  </si>
+  <si>
+    <t>Length 1 epoch</t>
+  </si>
+  <si>
+    <t>12-15min</t>
+  </si>
+  <si>
+    <t>12min</t>
+  </si>
+  <si>
+    <t>5-7 min</t>
+  </si>
+  <si>
+    <t>1-2 min</t>
+  </si>
+  <si>
+    <t>accuracy : 85%</t>
+  </si>
+  <si>
+    <t>model_10</t>
+  </si>
+  <si>
+    <t>resnet101</t>
+  </si>
+  <si>
+    <t>4-6 min</t>
+  </si>
+  <si>
+    <t>accuracy : 91%</t>
+  </si>
+  <si>
+    <t>EarlyStopping at epoch 7</t>
+  </si>
+  <si>
+    <t>non : (345-3=342)</t>
+  </si>
+  <si>
+    <t>model_11</t>
+  </si>
+  <si>
+    <t>accuracy : ?%</t>
+  </si>
+  <si>
+    <t>4-5 min</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="2"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -96,8 +257,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -412,77 +590,542 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B851BF5A-BEFD-554B-87CF-0C834BCAE8D6}">
-  <dimension ref="B2:H4"/>
+  <dimension ref="A2:R21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="M10" sqref="M10:M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.83203125" customWidth="1"/>
+    <col min="3" max="3" width="15.5" customWidth="1"/>
+    <col min="4" max="4" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.33203125" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" customWidth="1"/>
+    <col min="7" max="7" width="8.5" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" customWidth="1"/>
+    <col min="9" max="9" width="9" customWidth="1"/>
+    <col min="10" max="10" width="12.33203125" style="3" customWidth="1"/>
+    <col min="11" max="11" width="12.33203125" customWidth="1"/>
+    <col min="12" max="12" width="15" customWidth="1"/>
+    <col min="13" max="13" width="11.6640625" customWidth="1"/>
+    <col min="14" max="14" width="4.33203125" customWidth="1"/>
+    <col min="17" max="17" width="6.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O2" t="s">
+        <v>25</v>
+      </c>
+      <c r="R2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="1">
+        <v>50</v>
+      </c>
+      <c r="H3" s="1">
+        <v>5</v>
+      </c>
+      <c r="I3" s="1">
+        <v>500</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K3" s="1">
+        <v>16</v>
+      </c>
+      <c r="L3" s="1">
+        <v>84</v>
+      </c>
+      <c r="M3" s="1">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="1">
+        <v>50</v>
+      </c>
+      <c r="H4" s="1">
+        <v>5</v>
+      </c>
+      <c r="I4" s="1">
+        <v>500</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K4" s="1">
+        <v>16</v>
+      </c>
+      <c r="L4" s="1">
+        <v>90</v>
+      </c>
+      <c r="M4" s="1">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5">
+        <v>50</v>
+      </c>
+      <c r="H5">
+        <v>5</v>
+      </c>
+      <c r="I5">
+        <v>15000</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K5">
+        <v>16</v>
+      </c>
+      <c r="L5" s="8">
+        <v>0.84</v>
+      </c>
+      <c r="M5">
+        <v>1000</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="R5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6">
+        <v>20</v>
+      </c>
+      <c r="H6">
         <v>3</v>
       </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="I6">
+        <v>15000</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K6">
+        <v>32</v>
+      </c>
+      <c r="L6" s="8">
+        <v>0.84</v>
+      </c>
+      <c r="M6">
+        <v>1000</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="R6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" t="s">
         <v>1</v>
       </c>
-      <c r="D3" t="s">
+      <c r="C7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7">
         <v>10</v>
       </c>
-      <c r="E3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="H7">
+        <v>3</v>
+      </c>
+      <c r="I7">
+        <v>15000</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K7">
+        <v>32</v>
+      </c>
+      <c r="L7" s="9">
+        <v>0.85</v>
+      </c>
+      <c r="M7">
+        <v>1000</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="R7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="7"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="L9" s="3"/>
+      <c r="O9" s="2"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
         <v>8</v>
       </c>
-      <c r="H3">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="D10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10">
+        <v>10</v>
+      </c>
+      <c r="H10">
+        <v>3</v>
+      </c>
+      <c r="I10">
+        <v>50917</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K10">
+        <v>32</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="R10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" t="s">
         <v>1</v>
       </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="C11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11">
+        <v>10</v>
+      </c>
+      <c r="H11">
+        <v>3</v>
+      </c>
+      <c r="I11">
+        <v>50917</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K11">
+        <v>32</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="O11" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="R11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" t="s">
         <v>8</v>
       </c>
-      <c r="H4">
-        <v>90</v>
+      <c r="D13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" t="s">
+        <v>48</v>
+      </c>
+      <c r="F13" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13">
+        <v>10</v>
+      </c>
+      <c r="H13">
+        <v>3</v>
+      </c>
+      <c r="I13">
+        <v>50917</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K13">
+        <v>32</v>
+      </c>
+      <c r="L13" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="O13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="R13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" t="s">
+        <v>52</v>
+      </c>
+      <c r="F16" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16">
+        <v>10</v>
+      </c>
+      <c r="H16">
+        <v>3</v>
+      </c>
+      <c r="I16">
+        <v>50917</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K16">
+        <v>32</v>
+      </c>
+      <c r="L16" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="O16" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="R16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" t="s">
+        <v>56</v>
+      </c>
+      <c r="F17" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17">
+        <v>10</v>
+      </c>
+      <c r="H17">
+        <v>3</v>
+      </c>
+      <c r="I17">
+        <v>50917</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K17">
+        <v>32</v>
+      </c>
+      <c r="L17" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="R17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="G21" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>